<commit_message>
fix BOM Q1 model wrong
</commit_message>
<xml_diff>
--- a/Doc/Nebulizer_medical-立创商城报价.xlsx
+++ b/Doc/Nebulizer_medical-立创商城报价.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65cb10322f646d5c/Work/Nebulizer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/65cb10322f646d5c/Work/Nebulizer/PCB/Neblizer_medical/Doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{83932AD3-0008-48E3-8879-B6E1F6B9ED82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60BCD0D2-AA3B-4061-9482-EA7CC7A84D7E}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{83932AD3-0008-48E3-8879-B6E1F6B9ED82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CD68062-B911-4374-B73F-4644EC3B87A3}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{BD463D50-8921-400C-8C16-FCC09A4CBD35}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="508">
   <si>
     <t>Nebulizer_medical</t>
   </si>
@@ -964,33 +964,12 @@
     <t>Q1</t>
   </si>
   <si>
-    <t>IRL100HS121</t>
-  </si>
-  <si>
     <t>MOSFET (N-Channel)</t>
   </si>
   <si>
-    <t>Infineon(英飞凌)</t>
-  </si>
-  <si>
-    <t>PQFN-6-EP(2x2)</t>
-  </si>
-  <si>
     <t>三极管/MOS管/晶体管</t>
   </si>
   <si>
-    <t>C538106</t>
-  </si>
-  <si>
-    <t>https://item.szlcsc.com/558449.html</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>8.46</t>
-  </si>
-  <si>
     <t>Q2</t>
   </si>
   <si>
@@ -1553,7 +1532,7 @@
   </si>
   <si>
     <t>项目统计</t>
-    <phoneticPr fontId="125" type="noConversion"/>
+    <phoneticPr fontId="124" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -1569,23 +1548,36 @@
       </rPr>
       <t>总计：</t>
     </r>
-    <phoneticPr fontId="125" type="noConversion"/>
+    <phoneticPr fontId="124" type="noConversion"/>
   </si>
   <si>
     <t>C3, C6, C13, C14, C15, C16</t>
-    <phoneticPr fontId="125" type="noConversion"/>
+    <phoneticPr fontId="124" type="noConversion"/>
   </si>
   <si>
     <t>U4</t>
-    <phoneticPr fontId="125" type="noConversion"/>
+    <phoneticPr fontId="124" type="noConversion"/>
   </si>
   <si>
     <t>U2</t>
-    <phoneticPr fontId="125" type="noConversion"/>
+    <phoneticPr fontId="124" type="noConversion"/>
   </si>
   <si>
     <t>R1, R13, R27</t>
-    <phoneticPr fontId="125" type="noConversion"/>
+    <phoneticPr fontId="124" type="noConversion"/>
+  </si>
+  <si>
+    <t>FDN86246</t>
+  </si>
+  <si>
+    <t>SOT95P237X122-3N</t>
+  </si>
+  <si>
+    <t>C891118</t>
+  </si>
+  <si>
+    <t>https://item.szlcsc.com/956588.html?fromZone=s_s__%2522FDN86246%2522</t>
+    <phoneticPr fontId="124" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2148,14 +2140,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="10"/>
-      <color indexed="12"/>
-      <name val="微软雅黑"/>
-      <family val="2"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="微软雅黑"/>
       <family val="2"/>
@@ -2471,6 +2455,13 @@
       <b/>
       <u/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -2501,7 +2492,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -2553,11 +2544,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2787,127 +2790,124 @@
     <xf numFmtId="0" fontId="83" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="84" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="86" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="87" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="88" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="89" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="90" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="91" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="92" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="93" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="94" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="95" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="96" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="97" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="98" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="99" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="101" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="102" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="103" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="104" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="105" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="106" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="107" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="108" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="109" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="110" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="111" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="112" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="113" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="114" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="115" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="116" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="117" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="118" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="119" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="120" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="121" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="122" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="123" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="124" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="84" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="87" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="88" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="89" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="90" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="91" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="92" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="93" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="94" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="95" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="97" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="98" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="99" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="101" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="102" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="103" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="104" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="105" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="106" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="107" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="108" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="109" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="110" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="111" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="112" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="113" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="114" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="115" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="116" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="117" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="118" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="119" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="120" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="121" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="122" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="123" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2916,16 +2916,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="125" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="126" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="127" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="128" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2964,9 +2964,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3281,205 +3284,205 @@
   <dimension ref="A1:AC52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.6640625" style="118" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" style="118" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="118"/>
-    <col min="4" max="4" width="9.44140625" style="118" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="8.88671875" style="118"/>
-    <col min="8" max="8" width="13.109375" style="118" bestFit="1" customWidth="1"/>
-    <col min="9" max="20" width="8.88671875" style="118"/>
-    <col min="21" max="21" width="9.44140625" style="118" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.88671875" style="118"/>
-    <col min="23" max="23" width="7.5546875" style="118" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="8.88671875" style="118"/>
-    <col min="26" max="26" width="11.33203125" style="118" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.88671875" style="118"/>
-    <col min="28" max="28" width="13.6640625" style="118" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.77734375" style="119" bestFit="1" customWidth="1"/>
-    <col min="30" max="70" width="8.88671875" style="118"/>
-    <col min="71" max="71" width="17" style="118" customWidth="1"/>
-    <col min="72" max="72" width="10" style="118" customWidth="1"/>
-    <col min="73" max="79" width="8.88671875" style="118"/>
-    <col min="80" max="80" width="10" style="118" customWidth="1"/>
-    <col min="81" max="16384" width="8.88671875" style="118"/>
+    <col min="1" max="1" width="42.6640625" style="117" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" style="117" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="117" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="117" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="8.88671875" style="117"/>
+    <col min="8" max="8" width="13.109375" style="117" bestFit="1" customWidth="1"/>
+    <col min="9" max="20" width="8.88671875" style="117"/>
+    <col min="21" max="21" width="9.44140625" style="117" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.88671875" style="117"/>
+    <col min="23" max="23" width="7.5546875" style="117" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="8.88671875" style="117"/>
+    <col min="26" max="26" width="11.33203125" style="117" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="8.88671875" style="117"/>
+    <col min="28" max="28" width="13.6640625" style="117" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.77734375" style="118" bestFit="1" customWidth="1"/>
+    <col min="30" max="70" width="8.88671875" style="117"/>
+    <col min="71" max="71" width="17" style="117" customWidth="1"/>
+    <col min="72" max="72" width="10" style="117" customWidth="1"/>
+    <col min="73" max="79" width="8.88671875" style="117"/>
+    <col min="80" max="80" width="10" style="117" customWidth="1"/>
+    <col min="81" max="16384" width="8.88671875" style="117"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="131" t="s">
+      <c r="A1" s="130" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="126"/>
-      <c r="C1" s="126"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="133" t="s">
+      <c r="B1" s="125"/>
+      <c r="C1" s="125"/>
+      <c r="D1" s="125"/>
+      <c r="E1" s="126"/>
+      <c r="F1" s="132" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="128"/>
-      <c r="H1" s="128"/>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="128"/>
-      <c r="L1" s="128"/>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="128"/>
-      <c r="P1" s="128"/>
-      <c r="Q1" s="128"/>
-      <c r="R1" s="128"/>
-      <c r="S1" s="128"/>
-      <c r="T1" s="128"/>
-      <c r="U1" s="128"/>
-      <c r="V1" s="128"/>
-      <c r="W1" s="128"/>
-      <c r="X1" s="128"/>
-      <c r="Y1" s="128"/>
-      <c r="Z1" s="128"/>
-      <c r="AA1" s="129"/>
+      <c r="G1" s="127"/>
+      <c r="H1" s="127"/>
+      <c r="I1" s="127"/>
+      <c r="J1" s="127"/>
+      <c r="K1" s="127"/>
+      <c r="L1" s="127"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="127"/>
+      <c r="Q1" s="127"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="127"/>
+      <c r="V1" s="127"/>
+      <c r="W1" s="127"/>
+      <c r="X1" s="127"/>
+      <c r="Y1" s="127"/>
+      <c r="Z1" s="127"/>
+      <c r="AA1" s="128"/>
     </row>
     <row r="2" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="126"/>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
-      <c r="E2" s="127"/>
-      <c r="F2" s="134" t="s">
+      <c r="A2" s="125"/>
+      <c r="B2" s="125"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="133" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="134" t="s">
+      <c r="G2" s="127"/>
+      <c r="H2" s="127"/>
+      <c r="I2" s="127"/>
+      <c r="J2" s="128"/>
+      <c r="K2" s="133" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="128"/>
-      <c r="M2" s="128"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="125" t="s">
+      <c r="L2" s="127"/>
+      <c r="M2" s="127"/>
+      <c r="N2" s="128"/>
+      <c r="O2" s="124" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="126"/>
-      <c r="Q2" s="126"/>
-      <c r="R2" s="126"/>
-      <c r="S2" s="126"/>
-      <c r="T2" s="126"/>
-      <c r="U2" s="126"/>
-      <c r="V2" s="126"/>
-      <c r="W2" s="126"/>
-      <c r="X2" s="126"/>
-      <c r="Y2" s="126"/>
-      <c r="Z2" s="126"/>
-      <c r="AA2" s="127"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="125"/>
+      <c r="R2" s="125"/>
+      <c r="S2" s="125"/>
+      <c r="T2" s="125"/>
+      <c r="U2" s="125"/>
+      <c r="V2" s="125"/>
+      <c r="W2" s="125"/>
+      <c r="X2" s="125"/>
+      <c r="Y2" s="125"/>
+      <c r="Z2" s="125"/>
+      <c r="AA2" s="126"/>
     </row>
     <row r="3" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="126"/>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="127"/>
-      <c r="F3" s="134" t="s">
+      <c r="A3" s="125"/>
+      <c r="B3" s="125"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="126"/>
+      <c r="F3" s="133" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="128"/>
-      <c r="H3" s="128"/>
-      <c r="I3" s="128"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="134" t="s">
+      <c r="G3" s="127"/>
+      <c r="H3" s="127"/>
+      <c r="I3" s="127"/>
+      <c r="J3" s="128"/>
+      <c r="K3" s="133" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="128"/>
-      <c r="M3" s="128"/>
-      <c r="N3" s="129"/>
-      <c r="O3" s="126"/>
-      <c r="P3" s="126"/>
-      <c r="Q3" s="126"/>
-      <c r="R3" s="126"/>
-      <c r="S3" s="126"/>
-      <c r="T3" s="126"/>
-      <c r="U3" s="126"/>
-      <c r="V3" s="126"/>
-      <c r="W3" s="126"/>
-      <c r="X3" s="126"/>
-      <c r="Y3" s="126"/>
-      <c r="Z3" s="126"/>
-      <c r="AA3" s="127"/>
+      <c r="L3" s="127"/>
+      <c r="M3" s="127"/>
+      <c r="N3" s="128"/>
+      <c r="O3" s="125"/>
+      <c r="P3" s="125"/>
+      <c r="Q3" s="125"/>
+      <c r="R3" s="125"/>
+      <c r="S3" s="125"/>
+      <c r="T3" s="125"/>
+      <c r="U3" s="125"/>
+      <c r="V3" s="125"/>
+      <c r="W3" s="125"/>
+      <c r="X3" s="125"/>
+      <c r="Y3" s="125"/>
+      <c r="Z3" s="125"/>
+      <c r="AA3" s="126"/>
     </row>
     <row r="4" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="128"/>
-      <c r="B4" s="128"/>
-      <c r="C4" s="128"/>
-      <c r="D4" s="128"/>
-      <c r="E4" s="129"/>
-      <c r="F4" s="134" t="s">
+      <c r="A4" s="127"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="127"/>
+      <c r="D4" s="127"/>
+      <c r="E4" s="128"/>
+      <c r="F4" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="128"/>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="128"/>
-      <c r="L4" s="128"/>
-      <c r="M4" s="128"/>
-      <c r="N4" s="129"/>
-      <c r="O4" s="128"/>
-      <c r="P4" s="128"/>
-      <c r="Q4" s="128"/>
-      <c r="R4" s="128"/>
-      <c r="S4" s="128"/>
-      <c r="T4" s="128"/>
-      <c r="U4" s="128"/>
-      <c r="V4" s="128"/>
-      <c r="W4" s="128"/>
-      <c r="X4" s="128"/>
-      <c r="Y4" s="128"/>
-      <c r="Z4" s="128"/>
-      <c r="AA4" s="129"/>
+      <c r="G4" s="127"/>
+      <c r="H4" s="127"/>
+      <c r="I4" s="127"/>
+      <c r="J4" s="127"/>
+      <c r="K4" s="127"/>
+      <c r="L4" s="127"/>
+      <c r="M4" s="127"/>
+      <c r="N4" s="128"/>
+      <c r="O4" s="127"/>
+      <c r="P4" s="127"/>
+      <c r="Q4" s="127"/>
+      <c r="R4" s="127"/>
+      <c r="S4" s="127"/>
+      <c r="T4" s="127"/>
+      <c r="U4" s="127"/>
+      <c r="V4" s="127"/>
+      <c r="W4" s="127"/>
+      <c r="X4" s="127"/>
+      <c r="Y4" s="127"/>
+      <c r="Z4" s="127"/>
+      <c r="AA4" s="128"/>
     </row>
     <row r="5" spans="1:29" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="132" t="s">
+      <c r="A5" s="131" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="128"/>
-      <c r="C5" s="128"/>
-      <c r="D5" s="128"/>
-      <c r="E5" s="129"/>
-      <c r="F5" s="135" t="s">
+      <c r="B5" s="127"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="128"/>
+      <c r="F5" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="128"/>
-      <c r="H5" s="128"/>
-      <c r="I5" s="128"/>
-      <c r="J5" s="128"/>
-      <c r="K5" s="128"/>
-      <c r="L5" s="128"/>
-      <c r="M5" s="128"/>
-      <c r="N5" s="129"/>
-      <c r="O5" s="130" t="s">
+      <c r="G5" s="127"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="127"/>
+      <c r="K5" s="127"/>
+      <c r="L5" s="127"/>
+      <c r="M5" s="127"/>
+      <c r="N5" s="128"/>
+      <c r="O5" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="P5" s="128"/>
-      <c r="Q5" s="128"/>
-      <c r="R5" s="128"/>
-      <c r="S5" s="128"/>
-      <c r="T5" s="128"/>
-      <c r="U5" s="128"/>
-      <c r="V5" s="128"/>
-      <c r="W5" s="128"/>
-      <c r="X5" s="128"/>
-      <c r="Y5" s="128"/>
-      <c r="Z5" s="128"/>
-      <c r="AA5" s="129"/>
-      <c r="AC5" s="120" t="s">
-        <v>505</v>
+      <c r="P5" s="127"/>
+      <c r="Q5" s="127"/>
+      <c r="R5" s="127"/>
+      <c r="S5" s="127"/>
+      <c r="T5" s="127"/>
+      <c r="U5" s="127"/>
+      <c r="V5" s="127"/>
+      <c r="W5" s="127"/>
+      <c r="X5" s="127"/>
+      <c r="Y5" s="127"/>
+      <c r="Z5" s="127"/>
+      <c r="AA5" s="128"/>
+      <c r="AC5" s="119" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="15" x14ac:dyDescent="0.25">
@@ -3564,7 +3567,7 @@
       <c r="AA6" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="AC6" s="121"/>
+      <c r="AC6" s="120"/>
     </row>
     <row r="7" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
@@ -3648,7 +3651,7 @@
       <c r="AA7" s="29">
         <v>2.5299999999999998</v>
       </c>
-      <c r="AC7" s="121">
+      <c r="AC7" s="120">
         <f>W7*Z7</f>
         <v>0.12640000000000001</v>
       </c>
@@ -3735,7 +3738,7 @@
       <c r="AA8" s="29">
         <v>3.19</v>
       </c>
-      <c r="AC8" s="121">
+      <c r="AC8" s="120">
         <f t="shared" ref="AC8:AC49" si="0">W8*Z8</f>
         <v>0.31852000000000003</v>
       </c>
@@ -3822,7 +3825,7 @@
       <c r="AA9" s="29">
         <v>4.1500000000000004</v>
       </c>
-      <c r="AC9" s="121">
+      <c r="AC9" s="120">
         <f t="shared" si="0"/>
         <v>4.1466000000000003E-2</v>
       </c>
@@ -3909,14 +3912,14 @@
       <c r="AA10" s="29">
         <v>1.89</v>
       </c>
-      <c r="AC10" s="121">
+      <c r="AC10" s="120">
         <f t="shared" si="0"/>
         <v>3.7876E-2</v>
       </c>
     </row>
     <row r="11" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="124" t="s">
-        <v>507</v>
+      <c r="A11" s="123" t="s">
+        <v>500</v>
       </c>
       <c r="B11" s="28" t="s">
         <v>132</v>
@@ -3996,7 +3999,7 @@
       <c r="AA11" s="29">
         <v>1.53</v>
       </c>
-      <c r="AC11" s="121">
+      <c r="AC11" s="120">
         <f t="shared" si="0"/>
         <v>0.18359999999999999</v>
       </c>
@@ -4083,7 +4086,7 @@
       <c r="AA12" s="29">
         <v>4.16</v>
       </c>
-      <c r="AC12" s="121">
+      <c r="AC12" s="120">
         <f t="shared" si="0"/>
         <v>8.3139000000000005E-2</v>
       </c>
@@ -4170,7 +4173,7 @@
       <c r="AA13" s="29">
         <v>3.95</v>
       </c>
-      <c r="AC13" s="121">
+      <c r="AC13" s="120">
         <f t="shared" si="0"/>
         <v>3.9524999999999998E-2</v>
       </c>
@@ -4257,7 +4260,7 @@
       <c r="AA14" s="29">
         <v>2.86</v>
       </c>
-      <c r="AC14" s="121">
+      <c r="AC14" s="120">
         <f t="shared" si="0"/>
         <v>0.42833699999999997</v>
       </c>
@@ -4344,7 +4347,7 @@
       <c r="AA15" s="29">
         <v>2.86</v>
       </c>
-      <c r="AC15" s="121">
+      <c r="AC15" s="120">
         <f t="shared" si="0"/>
         <v>0.28555799999999998</v>
       </c>
@@ -4431,7 +4434,7 @@
       <c r="AA16" s="29">
         <v>4.5999999999999996</v>
       </c>
-      <c r="AC16" s="121">
+      <c r="AC16" s="120">
         <f t="shared" si="0"/>
         <v>4.6046999999999998E-2</v>
       </c>
@@ -4518,7 +4521,7 @@
       <c r="AA17" s="29">
         <v>1.53</v>
       </c>
-      <c r="AC17" s="121">
+      <c r="AC17" s="120">
         <f t="shared" si="0"/>
         <v>6.1199999999999997E-2</v>
       </c>
@@ -4605,7 +4608,7 @@
       <c r="AA18" s="29">
         <v>2.91</v>
       </c>
-      <c r="AC18" s="121">
+      <c r="AC18" s="120">
         <f t="shared" si="0"/>
         <v>5.8295E-2</v>
       </c>
@@ -4692,7 +4695,7 @@
       <c r="AA19" s="29">
         <v>3.01</v>
       </c>
-      <c r="AC19" s="121">
+      <c r="AC19" s="120">
         <f t="shared" si="0"/>
         <v>0.45081299999999996</v>
       </c>
@@ -4779,7 +4782,7 @@
       <c r="AA20" s="29">
         <v>2.13</v>
       </c>
-      <c r="AC20" s="121">
+      <c r="AC20" s="120">
         <f t="shared" si="0"/>
         <v>0.42605199999999999</v>
       </c>
@@ -4866,7 +4869,7 @@
       <c r="AA21" s="29">
         <v>3.05</v>
       </c>
-      <c r="AC21" s="121">
+      <c r="AC21" s="120">
         <f t="shared" si="0"/>
         <v>0.60960599999999998</v>
       </c>
@@ -4953,7 +4956,7 @@
       <c r="AA22" s="29">
         <v>6.15</v>
       </c>
-      <c r="AC22" s="121">
+      <c r="AC22" s="120">
         <f t="shared" si="0"/>
         <v>1.2302500000000001</v>
       </c>
@@ -5040,7 +5043,7 @@
       <c r="AA23" s="29">
         <v>1.69</v>
       </c>
-      <c r="AC23" s="121">
+      <c r="AC23" s="120">
         <f t="shared" si="0"/>
         <v>1.6850000000000001</v>
       </c>
@@ -5127,7 +5130,7 @@
       <c r="AA24" s="29">
         <v>4.3</v>
       </c>
-      <c r="AC24" s="121">
+      <c r="AC24" s="120">
         <f t="shared" si="0"/>
         <v>0.43024600000000002</v>
       </c>
@@ -5214,7 +5217,7 @@
       <c r="AA25" s="29">
         <v>2.0299999999999998</v>
       </c>
-      <c r="AC25" s="121">
+      <c r="AC25" s="120">
         <f t="shared" si="0"/>
         <v>0.14193900000000001</v>
       </c>
@@ -5301,7 +5304,7 @@
       <c r="AA26" s="29">
         <v>1.89</v>
       </c>
-      <c r="AC26" s="121">
+      <c r="AC26" s="120">
         <f t="shared" si="0"/>
         <v>1.8883E-2</v>
       </c>
@@ -5388,7 +5391,7 @@
       <c r="AA27" s="29">
         <v>2.78</v>
       </c>
-      <c r="AC27" s="121">
+      <c r="AC27" s="120">
         <f t="shared" si="0"/>
         <v>5.5669999999999997E-2</v>
       </c>
@@ -5397,50 +5400,34 @@
       <c r="A28" s="28" t="s">
         <v>308</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="135" t="s">
+        <v>504</v>
+      </c>
+      <c r="C28" s="135" t="s">
+        <v>505</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="135" t="s">
         <v>309</v>
       </c>
-      <c r="C28" s="28" t="s">
-        <v>309</v>
-      </c>
-      <c r="D28" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="28" t="s">
+      <c r="F28" s="76"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28" t="s">
         <v>310</v>
       </c>
-      <c r="F28" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="G28" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="H28" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="I28" s="28" t="s">
-        <v>309</v>
-      </c>
-      <c r="J28" s="28" t="s">
-        <v>309</v>
-      </c>
-      <c r="K28" s="28" t="s">
-        <v>311</v>
-      </c>
-      <c r="L28" s="28" t="s">
-        <v>312</v>
-      </c>
-      <c r="M28" s="28" t="s">
-        <v>43</v>
-      </c>
-      <c r="N28" s="28" t="s">
-        <v>313</v>
-      </c>
       <c r="O28" s="28" t="s">
-        <v>314</v>
-      </c>
-      <c r="P28" s="77" t="s">
-        <v>315</v>
+        <v>506</v>
+      </c>
+      <c r="P28" s="136" t="s">
+        <v>507</v>
       </c>
       <c r="Q28" s="28" t="s">
         <v>53</v>
@@ -5451,9 +5438,7 @@
       <c r="S28" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="T28" s="28" t="s">
-        <v>72</v>
-      </c>
+      <c r="T28" s="28"/>
       <c r="U28" s="28" t="s">
         <v>77</v>
       </c>
@@ -5463,40 +5448,38 @@
       <c r="W28" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="X28" s="28" t="s">
-        <v>316</v>
-      </c>
+      <c r="X28" s="28"/>
       <c r="Y28" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="Z28" s="28" t="s">
-        <v>317</v>
+      <c r="Z28" s="28">
+        <v>3.78</v>
       </c>
       <c r="AA28" s="29">
-        <v>8.4600000000000009</v>
-      </c>
-      <c r="AC28" s="121">
+        <v>3.78</v>
+      </c>
+      <c r="AC28" s="120">
         <f t="shared" si="0"/>
-        <v>8.4600000000000009</v>
+        <v>3.78</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D29" s="28" t="s">
         <v>77</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>321</v>
-      </c>
-      <c r="F29" s="78" t="s">
+        <v>314</v>
+      </c>
+      <c r="F29" s="77" t="s">
         <v>42</v>
       </c>
       <c r="G29" s="28" t="s">
@@ -5506,28 +5489,28 @@
         <v>215</v>
       </c>
       <c r="I29" s="28" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="J29" s="28" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="K29" s="28" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="L29" s="28" t="s">
         <v>177</v>
       </c>
       <c r="M29" s="28" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="N29" s="28" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="O29" s="28" t="s">
-        <v>326</v>
-      </c>
-      <c r="P29" s="79" t="s">
-        <v>327</v>
+        <v>319</v>
+      </c>
+      <c r="P29" s="78" t="s">
+        <v>320</v>
       </c>
       <c r="Q29" s="28" t="s">
         <v>53</v>
@@ -5551,28 +5534,28 @@
         <v>77</v>
       </c>
       <c r="X29" s="28" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="Y29" s="28" t="s">
         <v>40</v>
       </c>
       <c r="Z29" s="28" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="AA29" s="29">
         <v>1.7</v>
       </c>
-      <c r="AC29" s="121">
+      <c r="AC29" s="120">
         <f t="shared" si="0"/>
         <v>0.33950200000000003</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C30" s="28" t="s">
         <v>174</v>
@@ -5581,9 +5564,9 @@
         <v>77</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>332</v>
-      </c>
-      <c r="F30" s="80" t="s">
+        <v>325</v>
+      </c>
+      <c r="F30" s="79" t="s">
         <v>91</v>
       </c>
       <c r="G30" s="28" t="s">
@@ -5593,28 +5576,28 @@
         <v>200</v>
       </c>
       <c r="I30" s="28" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="K30" s="28" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="L30" s="28" t="s">
         <v>177</v>
       </c>
       <c r="M30" s="28" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="N30" s="28" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="O30" s="28" t="s">
-        <v>336</v>
-      </c>
-      <c r="P30" s="81" t="s">
-        <v>337</v>
+        <v>329</v>
+      </c>
+      <c r="P30" s="80" t="s">
+        <v>330</v>
       </c>
       <c r="Q30" s="28" t="s">
         <v>53</v>
@@ -5638,31 +5621,31 @@
         <v>77</v>
       </c>
       <c r="X30" s="28" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="Y30" s="28" t="s">
         <v>208</v>
       </c>
       <c r="Z30" s="28" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="AA30" s="29">
         <v>2.56</v>
       </c>
-      <c r="AC30" s="121">
+      <c r="AC30" s="120">
         <f t="shared" si="0"/>
         <v>0.25616499999999998</v>
       </c>
     </row>
     <row r="31" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="124" t="s">
-        <v>510</v>
+      <c r="A31" s="123" t="s">
+        <v>503</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D31" s="28" t="s">
         <v>102</v>
@@ -5670,38 +5653,38 @@
       <c r="E31" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F31" s="82" t="s">
+      <c r="F31" s="81" t="s">
         <v>91</v>
       </c>
       <c r="G31" s="28" t="s">
         <v>43</v>
       </c>
       <c r="H31" s="28" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="I31" s="28" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="J31" s="28" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="K31" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L31" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M31" s="28" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="N31" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O31" s="28" t="s">
-        <v>348</v>
-      </c>
-      <c r="P31" s="83" t="s">
-        <v>349</v>
+        <v>341</v>
+      </c>
+      <c r="P31" s="82" t="s">
+        <v>342</v>
       </c>
       <c r="Q31" s="28" t="s">
         <v>53</v>
@@ -5725,70 +5708,70 @@
         <v>3</v>
       </c>
       <c r="X31" s="28" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="Y31" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z31" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="AA31" s="29">
         <v>0.31</v>
       </c>
-      <c r="AC31" s="121">
+      <c r="AC31" s="120">
         <f t="shared" si="0"/>
         <v>9.333000000000001E-3</v>
       </c>
     </row>
     <row r="32" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="E32" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="84" t="s">
+      <c r="F32" s="83" t="s">
         <v>42</v>
       </c>
       <c r="G32" s="28" t="s">
         <v>43</v>
       </c>
       <c r="H32" s="28" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="I32" s="28" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="J32" s="28" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="K32" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L32" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M32" s="28" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="N32" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O32" s="28" t="s">
-        <v>359</v>
-      </c>
-      <c r="P32" s="85" t="s">
-        <v>360</v>
+        <v>352</v>
+      </c>
+      <c r="P32" s="84" t="s">
+        <v>353</v>
       </c>
       <c r="Q32" s="28" t="s">
         <v>53</v>
@@ -5803,40 +5786,40 @@
         <v>56</v>
       </c>
       <c r="U32" s="28" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="V32" s="28" t="s">
         <v>57</v>
       </c>
       <c r="W32" s="28" t="s">
+        <v>347</v>
+      </c>
+      <c r="X32" s="28" t="s">
         <v>354</v>
-      </c>
-      <c r="X32" s="28" t="s">
-        <v>361</v>
       </c>
       <c r="Y32" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z32" s="28" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="AA32" s="29">
         <v>0.38</v>
       </c>
-      <c r="AC32" s="121">
+      <c r="AC32" s="120">
         <f t="shared" si="0"/>
         <v>3.3785999999999997E-2</v>
       </c>
     </row>
     <row r="33" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D33" s="28" t="s">
         <v>63</v>
@@ -5844,7 +5827,7 @@
       <c r="E33" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F33" s="86" t="s">
+      <c r="F33" s="85" t="s">
         <v>42</v>
       </c>
       <c r="G33" s="28" t="s">
@@ -5854,28 +5837,28 @@
         <v>92</v>
       </c>
       <c r="I33" s="28" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="J33" s="28" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="K33" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L33" s="28" t="s">
         <v>76</v>
       </c>
       <c r="M33" s="28" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="N33" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O33" s="28" t="s">
-        <v>369</v>
-      </c>
-      <c r="P33" s="87" t="s">
-        <v>370</v>
+        <v>362</v>
+      </c>
+      <c r="P33" s="86" t="s">
+        <v>363</v>
       </c>
       <c r="Q33" s="28" t="s">
         <v>53</v>
@@ -5887,7 +5870,7 @@
         <v>55</v>
       </c>
       <c r="T33" s="28" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="U33" s="28" t="s">
         <v>63</v>
@@ -5899,31 +5882,31 @@
         <v>63</v>
       </c>
       <c r="X33" s="28" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="Y33" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z33" s="28" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="AA33" s="29">
         <v>0.66</v>
       </c>
-      <c r="AC33" s="121">
+      <c r="AC33" s="120">
         <f t="shared" si="0"/>
         <v>1.3103999999999999E-2</v>
       </c>
     </row>
     <row r="34" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D34" s="28" t="s">
         <v>77</v>
@@ -5931,7 +5914,7 @@
       <c r="E34" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F34" s="88" t="s">
+      <c r="F34" s="87" t="s">
         <v>91</v>
       </c>
       <c r="G34" s="28" t="s">
@@ -5941,28 +5924,28 @@
         <v>79</v>
       </c>
       <c r="I34" s="28" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="J34" s="28" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="K34" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L34" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M34" s="28" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="N34" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O34" s="28" t="s">
-        <v>379</v>
-      </c>
-      <c r="P34" s="89" t="s">
-        <v>380</v>
+        <v>372</v>
+      </c>
+      <c r="P34" s="88" t="s">
+        <v>373</v>
       </c>
       <c r="Q34" s="28" t="s">
         <v>53</v>
@@ -5986,31 +5969,31 @@
         <v>77</v>
       </c>
       <c r="X34" s="28" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="Y34" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z34" s="28" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="AA34" s="29">
         <v>0.39</v>
       </c>
-      <c r="AC34" s="121">
+      <c r="AC34" s="120">
         <f t="shared" si="0"/>
         <v>3.8660000000000001E-3</v>
       </c>
     </row>
     <row r="35" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D35" s="28" t="s">
         <v>77</v>
@@ -6018,7 +6001,7 @@
       <c r="E35" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="90" t="s">
+      <c r="F35" s="89" t="s">
         <v>91</v>
       </c>
       <c r="G35" s="28" t="s">
@@ -6028,28 +6011,28 @@
         <v>79</v>
       </c>
       <c r="I35" s="28" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="J35" s="28" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="K35" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L35" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M35" s="28" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="N35" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O35" s="28" t="s">
-        <v>348</v>
-      </c>
-      <c r="P35" s="91" t="s">
-        <v>349</v>
+        <v>341</v>
+      </c>
+      <c r="P35" s="90" t="s">
+        <v>342</v>
       </c>
       <c r="Q35" s="28" t="s">
         <v>53</v>
@@ -6073,31 +6056,31 @@
         <v>77</v>
       </c>
       <c r="X35" s="28" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="Y35" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z35" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="AA35" s="29">
         <v>0.31</v>
       </c>
-      <c r="AC35" s="121">
+      <c r="AC35" s="120">
         <f t="shared" si="0"/>
         <v>3.1110000000000001E-3</v>
       </c>
     </row>
     <row r="36" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D36" s="28" t="s">
         <v>77</v>
@@ -6105,7 +6088,7 @@
       <c r="E36" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F36" s="92" t="s">
+      <c r="F36" s="91" t="s">
         <v>42</v>
       </c>
       <c r="G36" s="28" t="s">
@@ -6115,28 +6098,28 @@
         <v>79</v>
       </c>
       <c r="I36" s="28" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="J36" s="28" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="K36" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L36" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M36" s="28" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="N36" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O36" s="28" t="s">
-        <v>390</v>
-      </c>
-      <c r="P36" s="93" t="s">
-        <v>391</v>
+        <v>383</v>
+      </c>
+      <c r="P36" s="92" t="s">
+        <v>384</v>
       </c>
       <c r="Q36" s="28" t="s">
         <v>53</v>
@@ -6160,31 +6143,31 @@
         <v>77</v>
       </c>
       <c r="X36" s="28" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="Y36" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z36" s="28" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="AA36" s="29">
         <v>0.86</v>
       </c>
-      <c r="AC36" s="121">
+      <c r="AC36" s="120">
         <f t="shared" si="0"/>
         <v>8.6429999999999996E-3</v>
       </c>
     </row>
     <row r="37" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D37" s="28" t="s">
         <v>63</v>
@@ -6192,7 +6175,7 @@
       <c r="E37" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F37" s="94" t="s">
+      <c r="F37" s="93" t="s">
         <v>42</v>
       </c>
       <c r="G37" s="28" t="s">
@@ -6202,28 +6185,28 @@
         <v>92</v>
       </c>
       <c r="I37" s="28" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="J37" s="28" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="K37" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L37" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M37" s="28" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="N37" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O37" s="28" t="s">
-        <v>399</v>
-      </c>
-      <c r="P37" s="95" t="s">
-        <v>400</v>
+        <v>392</v>
+      </c>
+      <c r="P37" s="94" t="s">
+        <v>393</v>
       </c>
       <c r="Q37" s="28" t="s">
         <v>53</v>
@@ -6247,31 +6230,31 @@
         <v>63</v>
       </c>
       <c r="X37" s="28" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="Y37" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z37" s="28" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="AA37" s="29">
         <v>0.34</v>
       </c>
-      <c r="AC37" s="121">
+      <c r="AC37" s="120">
         <f t="shared" si="0"/>
         <v>6.7520000000000002E-3</v>
       </c>
     </row>
     <row r="38" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="B38" s="28" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D38" s="28" t="s">
         <v>63</v>
@@ -6279,7 +6262,7 @@
       <c r="E38" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F38" s="96" t="s">
+      <c r="F38" s="95" t="s">
         <v>91</v>
       </c>
       <c r="G38" s="28" t="s">
@@ -6289,28 +6272,28 @@
         <v>92</v>
       </c>
       <c r="I38" s="28" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="J38" s="28" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="K38" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L38" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M38" s="28" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="N38" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O38" s="28" t="s">
-        <v>408</v>
-      </c>
-      <c r="P38" s="97" t="s">
-        <v>409</v>
+        <v>401</v>
+      </c>
+      <c r="P38" s="96" t="s">
+        <v>402</v>
       </c>
       <c r="Q38" s="28" t="s">
         <v>53</v>
@@ -6334,39 +6317,39 @@
         <v>63</v>
       </c>
       <c r="X38" s="28" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="Y38" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z38" s="28" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="AA38" s="29">
         <v>0.38</v>
       </c>
-      <c r="AC38" s="121">
+      <c r="AC38" s="120">
         <f t="shared" si="0"/>
         <v>7.6579999999999999E-3</v>
       </c>
     </row>
     <row r="39" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="B39" s="28" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D39" s="28" t="s">
         <v>63</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>414</v>
-      </c>
-      <c r="F39" s="98" t="s">
+        <v>407</v>
+      </c>
+      <c r="F39" s="97" t="s">
         <v>42</v>
       </c>
       <c r="G39" s="28" t="s">
@@ -6376,28 +6359,28 @@
         <v>92</v>
       </c>
       <c r="I39" s="28" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="J39" s="28" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="K39" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L39" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M39" s="28" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="N39" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O39" s="28" t="s">
-        <v>418</v>
-      </c>
-      <c r="P39" s="99" t="s">
-        <v>419</v>
+        <v>411</v>
+      </c>
+      <c r="P39" s="98" t="s">
+        <v>412</v>
       </c>
       <c r="Q39" s="28" t="s">
         <v>53</v>
@@ -6421,31 +6404,31 @@
         <v>63</v>
       </c>
       <c r="X39" s="28" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="Y39" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z39" s="28" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="AA39" s="29">
         <v>0.39</v>
       </c>
-      <c r="AC39" s="121">
+      <c r="AC39" s="120">
         <f t="shared" si="0"/>
         <v>7.7159999999999998E-3</v>
       </c>
     </row>
     <row r="40" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="B40" s="28" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D40" s="28" t="s">
         <v>63</v>
@@ -6453,7 +6436,7 @@
       <c r="E40" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="F40" s="100" t="s">
+      <c r="F40" s="99" t="s">
         <v>42</v>
       </c>
       <c r="G40" s="28" t="s">
@@ -6463,28 +6446,28 @@
         <v>92</v>
       </c>
       <c r="I40" s="28" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="J40" s="28" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="K40" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L40" s="28" t="s">
         <v>76</v>
       </c>
       <c r="M40" s="28" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="N40" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O40" s="28" t="s">
-        <v>427</v>
-      </c>
-      <c r="P40" s="101" t="s">
-        <v>428</v>
+        <v>420</v>
+      </c>
+      <c r="P40" s="100" t="s">
+        <v>421</v>
       </c>
       <c r="Q40" s="28" t="s">
         <v>53</v>
@@ -6496,7 +6479,7 @@
         <v>55</v>
       </c>
       <c r="T40" s="28" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="U40" s="28" t="s">
         <v>63</v>
@@ -6508,31 +6491,31 @@
         <v>63</v>
       </c>
       <c r="X40" s="28" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="Y40" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z40" s="28" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="AA40" s="29">
         <v>0.74</v>
       </c>
-      <c r="AC40" s="121">
+      <c r="AC40" s="120">
         <f t="shared" si="0"/>
         <v>1.4836E-2</v>
       </c>
     </row>
     <row r="41" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="B41" s="28" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D41" s="28" t="s">
         <v>63</v>
@@ -6540,7 +6523,7 @@
       <c r="E41" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F41" s="102" t="s">
+      <c r="F41" s="101" t="s">
         <v>91</v>
       </c>
       <c r="G41" s="28" t="s">
@@ -6550,28 +6533,28 @@
         <v>92</v>
       </c>
       <c r="I41" s="28" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="J41" s="28" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="K41" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L41" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M41" s="28" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="N41" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O41" s="28" t="s">
-        <v>348</v>
-      </c>
-      <c r="P41" s="103" t="s">
-        <v>349</v>
+        <v>341</v>
+      </c>
+      <c r="P41" s="102" t="s">
+        <v>342</v>
       </c>
       <c r="Q41" s="28" t="s">
         <v>53</v>
@@ -6595,39 +6578,39 @@
         <v>63</v>
       </c>
       <c r="X41" s="28" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="Y41" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z41" s="28" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="AA41" s="29">
         <v>0.31</v>
       </c>
-      <c r="AC41" s="121">
+      <c r="AC41" s="120">
         <f t="shared" si="0"/>
         <v>6.2220000000000001E-3</v>
       </c>
     </row>
     <row r="42" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="B42" s="28" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C42" s="28" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="D42" s="28" t="s">
         <v>77</v>
       </c>
       <c r="E42" s="28" t="s">
-        <v>435</v>
-      </c>
-      <c r="F42" s="104" t="s">
+        <v>428</v>
+      </c>
+      <c r="F42" s="103" t="s">
         <v>91</v>
       </c>
       <c r="G42" s="28" t="s">
@@ -6637,28 +6620,28 @@
         <v>79</v>
       </c>
       <c r="I42" s="28" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="J42" s="28" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="K42" s="28" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="L42" s="28" t="s">
         <v>76</v>
       </c>
       <c r="M42" s="28" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="N42" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O42" s="28" t="s">
-        <v>439</v>
-      </c>
-      <c r="P42" s="105" t="s">
-        <v>440</v>
+        <v>432</v>
+      </c>
+      <c r="P42" s="104" t="s">
+        <v>433</v>
       </c>
       <c r="Q42" s="28" t="s">
         <v>53</v>
@@ -6670,7 +6653,7 @@
         <v>55</v>
       </c>
       <c r="T42" s="28" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="U42" s="28" t="s">
         <v>77</v>
@@ -6682,31 +6665,31 @@
         <v>77</v>
       </c>
       <c r="X42" s="28" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="Y42" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z42" s="28" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="AA42" s="29">
         <v>2.0699999999999998</v>
       </c>
-      <c r="AC42" s="121">
+      <c r="AC42" s="120">
         <f t="shared" si="0"/>
         <v>2.0681000000000001E-2</v>
       </c>
     </row>
     <row r="43" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="B43" s="28" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D43" s="28" t="s">
         <v>77</v>
@@ -6714,7 +6697,7 @@
       <c r="E43" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="F43" s="106" t="s">
+      <c r="F43" s="105" t="s">
         <v>91</v>
       </c>
       <c r="G43" s="28" t="s">
@@ -6724,28 +6707,28 @@
         <v>79</v>
       </c>
       <c r="I43" s="28" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="J43" s="28" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="K43" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L43" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M43" s="28" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="N43" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O43" s="28" t="s">
-        <v>448</v>
-      </c>
-      <c r="P43" s="107" t="s">
-        <v>449</v>
+        <v>441</v>
+      </c>
+      <c r="P43" s="106" t="s">
+        <v>442</v>
       </c>
       <c r="Q43" s="28" t="s">
         <v>53</v>
@@ -6769,39 +6752,39 @@
         <v>77</v>
       </c>
       <c r="X43" s="28" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="Y43" s="28" t="s">
         <v>55</v>
       </c>
       <c r="Z43" s="28" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="AA43" s="29">
         <v>0.4</v>
       </c>
-      <c r="AC43" s="121">
+      <c r="AC43" s="120">
         <f t="shared" si="0"/>
         <v>3.9899999999999996E-3</v>
       </c>
     </row>
     <row r="44" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="B44" s="28" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D44" s="28" t="s">
         <v>63</v>
       </c>
       <c r="E44" s="28" t="s">
-        <v>454</v>
-      </c>
-      <c r="F44" s="108" t="s">
+        <v>447</v>
+      </c>
+      <c r="F44" s="107" t="s">
         <v>42</v>
       </c>
       <c r="G44" s="28" t="s">
@@ -6811,28 +6794,28 @@
         <v>134</v>
       </c>
       <c r="I44" s="28" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="J44" s="28" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="K44" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L44" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M44" s="28" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="N44" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O44" s="28" t="s">
-        <v>458</v>
-      </c>
-      <c r="P44" s="109" t="s">
-        <v>459</v>
+        <v>451</v>
+      </c>
+      <c r="P44" s="108" t="s">
+        <v>452</v>
       </c>
       <c r="Q44" s="28" t="s">
         <v>53</v>
@@ -6856,39 +6839,39 @@
         <v>63</v>
       </c>
       <c r="X44" s="28" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
       <c r="Y44" s="28" t="s">
         <v>110</v>
       </c>
       <c r="Z44" s="28" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
       <c r="AA44" s="29">
         <v>5.56</v>
       </c>
-      <c r="AC44" s="121">
+      <c r="AC44" s="120">
         <f t="shared" si="0"/>
         <v>0.22226799999999999</v>
       </c>
     </row>
     <row r="45" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
       <c r="C45" s="28" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D45" s="28" t="s">
         <v>63</v>
       </c>
       <c r="E45" s="28" t="s">
-        <v>454</v>
-      </c>
-      <c r="F45" s="110" t="s">
+        <v>447</v>
+      </c>
+      <c r="F45" s="109" t="s">
         <v>42</v>
       </c>
       <c r="G45" s="28" t="s">
@@ -6898,28 +6881,28 @@
         <v>134</v>
       </c>
       <c r="I45" s="28" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="J45" s="28" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="K45" s="28" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="L45" s="28" t="s">
         <v>48</v>
       </c>
       <c r="M45" s="28" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="N45" s="28" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="O45" s="28" t="s">
-        <v>467</v>
-      </c>
-      <c r="P45" s="111" t="s">
-        <v>468</v>
+        <v>460</v>
+      </c>
+      <c r="P45" s="110" t="s">
+        <v>461</v>
       </c>
       <c r="Q45" s="28" t="s">
         <v>53</v>
@@ -6943,39 +6926,39 @@
         <v>63</v>
       </c>
       <c r="X45" s="28" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="Y45" s="28" t="s">
         <v>110</v>
       </c>
       <c r="Z45" s="28" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="AA45" s="29">
         <v>6.4</v>
       </c>
-      <c r="AC45" s="121">
+      <c r="AC45" s="120">
         <f t="shared" si="0"/>
         <v>0.25615599999999999</v>
       </c>
     </row>
     <row r="46" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="B46" s="28" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="C46" s="28" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="D46" s="28" t="s">
         <v>77</v>
       </c>
       <c r="E46" s="28" t="s">
-        <v>474</v>
-      </c>
-      <c r="F46" s="112" t="s">
+        <v>467</v>
+      </c>
+      <c r="F46" s="111" t="s">
         <v>91</v>
       </c>
       <c r="G46" s="28" t="s">
@@ -6985,28 +6968,28 @@
         <v>116</v>
       </c>
       <c r="I46" s="28" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="J46" s="28" t="s">
+        <v>465</v>
+      </c>
+      <c r="K46" s="28" t="s">
+        <v>469</v>
+      </c>
+      <c r="L46" s="28" t="s">
+        <v>470</v>
+      </c>
+      <c r="M46" s="28" t="s">
+        <v>471</v>
+      </c>
+      <c r="N46" s="28" t="s">
         <v>472</v>
       </c>
-      <c r="K46" s="28" t="s">
-        <v>476</v>
-      </c>
-      <c r="L46" s="28" t="s">
-        <v>477</v>
-      </c>
-      <c r="M46" s="28" t="s">
-        <v>478</v>
-      </c>
-      <c r="N46" s="28" t="s">
-        <v>479</v>
-      </c>
       <c r="O46" s="28" t="s">
-        <v>480</v>
-      </c>
-      <c r="P46" s="113" t="s">
-        <v>481</v>
+        <v>473</v>
+      </c>
+      <c r="P46" s="112" t="s">
+        <v>474</v>
       </c>
       <c r="Q46" s="28" t="s">
         <v>53</v>
@@ -7018,7 +7001,7 @@
         <v>110</v>
       </c>
       <c r="T46" s="28" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="U46" s="28" t="s">
         <v>77</v>
@@ -7030,39 +7013,39 @@
         <v>77</v>
       </c>
       <c r="X46" s="28" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="Y46" s="28" t="s">
         <v>110</v>
       </c>
       <c r="Z46" s="28" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="AA46" s="29">
         <v>6.26</v>
       </c>
-      <c r="AC46" s="121">
+      <c r="AC46" s="120">
         <f t="shared" si="0"/>
         <v>0.125162</v>
       </c>
     </row>
     <row r="47" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
       <c r="B47" s="28" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="C47" s="28" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="D47" s="28" t="s">
         <v>77</v>
       </c>
       <c r="E47" s="28" t="s">
-        <v>487</v>
-      </c>
-      <c r="F47" s="114" t="s">
+        <v>480</v>
+      </c>
+      <c r="F47" s="113" t="s">
         <v>91</v>
       </c>
       <c r="G47" s="28" t="s">
@@ -7072,28 +7055,28 @@
         <v>215</v>
       </c>
       <c r="I47" s="28" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="J47" s="28" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="K47" s="28" t="s">
-        <v>488</v>
+        <v>481</v>
       </c>
       <c r="L47" s="28" t="s">
         <v>203</v>
       </c>
       <c r="M47" s="28" t="s">
-        <v>489</v>
+        <v>482</v>
       </c>
       <c r="N47" s="28" t="s">
-        <v>490</v>
+        <v>483</v>
       </c>
       <c r="O47" s="28" t="s">
-        <v>491</v>
-      </c>
-      <c r="P47" s="115" t="s">
-        <v>492</v>
+        <v>484</v>
+      </c>
+      <c r="P47" s="114" t="s">
+        <v>485</v>
       </c>
       <c r="Q47" s="28" t="s">
         <v>53</v>
@@ -7117,25 +7100,25 @@
         <v>77</v>
       </c>
       <c r="X47" s="28" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="Y47" s="28" t="s">
         <v>40</v>
       </c>
       <c r="Z47" s="28" t="s">
-        <v>493</v>
+        <v>486</v>
       </c>
       <c r="AA47" s="29">
         <v>9.27</v>
       </c>
-      <c r="AC47" s="121">
+      <c r="AC47" s="120">
         <f t="shared" si="0"/>
         <v>1.8531</v>
       </c>
     </row>
     <row r="48" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="124" t="s">
-        <v>509</v>
+      <c r="A48" s="123" t="s">
+        <v>502</v>
       </c>
       <c r="B48" s="28" t="s">
         <v>198</v>
@@ -7215,28 +7198,28 @@
       <c r="AA48" s="29">
         <v>2.81</v>
       </c>
-      <c r="AC48" s="121">
+      <c r="AC48" s="120">
         <f>W48*Z48</f>
         <v>0.28083399999999997</v>
       </c>
     </row>
     <row r="49" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="28" t="s">
-        <v>494</v>
+        <v>487</v>
       </c>
       <c r="B49" s="28" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>496</v>
+        <v>489</v>
       </c>
       <c r="D49" s="28" t="s">
         <v>77</v>
       </c>
       <c r="E49" s="28" t="s">
-        <v>497</v>
-      </c>
-      <c r="F49" s="116" t="s">
+        <v>490</v>
+      </c>
+      <c r="F49" s="115" t="s">
         <v>91</v>
       </c>
       <c r="G49" s="28" t="s">
@@ -7246,28 +7229,28 @@
         <v>215</v>
       </c>
       <c r="I49" s="28" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="J49" s="28" t="s">
-        <v>495</v>
+        <v>488</v>
       </c>
       <c r="K49" s="28" t="s">
-        <v>498</v>
+        <v>491</v>
       </c>
       <c r="L49" s="28" t="s">
-        <v>499</v>
+        <v>492</v>
       </c>
       <c r="M49" s="28" t="s">
-        <v>500</v>
+        <v>493</v>
       </c>
       <c r="N49" s="28" t="s">
         <v>205</v>
       </c>
       <c r="O49" s="28" t="s">
-        <v>501</v>
-      </c>
-      <c r="P49" s="117" t="s">
-        <v>502</v>
+        <v>494</v>
+      </c>
+      <c r="P49" s="116" t="s">
+        <v>495</v>
       </c>
       <c r="Q49" s="28" t="s">
         <v>53</v>
@@ -7291,25 +7274,25 @@
         <v>77</v>
       </c>
       <c r="X49" s="28" t="s">
-        <v>503</v>
+        <v>496</v>
       </c>
       <c r="Y49" s="28" t="s">
         <v>40</v>
       </c>
       <c r="Z49" s="28" t="s">
-        <v>504</v>
+        <v>497</v>
       </c>
       <c r="AA49" s="29">
         <v>2.4300000000000002</v>
       </c>
-      <c r="AC49" s="121">
+      <c r="AC49" s="120">
         <f t="shared" si="0"/>
         <v>0.485489</v>
       </c>
     </row>
     <row r="50" spans="1:29" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="124" t="s">
-        <v>508</v>
+      <c r="A50" s="123" t="s">
+        <v>501</v>
       </c>
       <c r="B50" s="28" t="s">
         <v>184</v>
@@ -7389,21 +7372,21 @@
       <c r="AA50" s="29">
         <v>8.4700000000000006</v>
       </c>
-      <c r="AC50" s="121">
+      <c r="AC50" s="120">
         <f>W50*Z50</f>
         <v>8.4668620000000008</v>
       </c>
     </row>
     <row r="51" spans="1:29" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="AC51" s="121"/>
+      <c r="AC51" s="120"/>
     </row>
     <row r="52" spans="1:29" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="AB52" s="123" t="s">
-        <v>506</v>
-      </c>
-      <c r="AC52" s="122">
+      <c r="AB52" s="122" t="s">
+        <v>499</v>
+      </c>
+      <c r="AC52" s="121">
         <f>SUM(AC7:AC49)</f>
-        <v>19.176796</v>
+        <v>14.496795999999998</v>
       </c>
     </row>
   </sheetData>
@@ -7420,7 +7403,7 @@
     <mergeCell ref="K2:N2"/>
     <mergeCell ref="K3:N3"/>
   </mergeCells>
-  <phoneticPr fontId="125" type="noConversion"/>
+  <phoneticPr fontId="124" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="P7" r:id="rId1" display="url" xr:uid="{7F028AB9-FE12-4BE3-9AD3-6ACC911E46F8}"/>
     <hyperlink ref="P8" r:id="rId2" display="url" xr:uid="{A8E5760E-7687-4727-8D5A-9ED6D61497B1}"/>
@@ -7445,30 +7428,30 @@
     <hyperlink ref="P25" r:id="rId21" display="url" xr:uid="{3F2BDA81-50FB-434D-9DDF-73F8B2DA29E9}"/>
     <hyperlink ref="P26" r:id="rId22" display="url" xr:uid="{2CA0685B-6A0A-4C50-BA5B-C177527A05D2}"/>
     <hyperlink ref="P27" r:id="rId23" display="url" xr:uid="{2C1BBB5C-1E1D-4260-98C6-47B3EA30F216}"/>
-    <hyperlink ref="P28" r:id="rId24" display="url" xr:uid="{8305FC19-A57E-42B1-BBCA-EC2164949609}"/>
-    <hyperlink ref="P29" r:id="rId25" display="url" xr:uid="{06A4437F-89A2-4876-AD94-331DFFE2053D}"/>
-    <hyperlink ref="P30" r:id="rId26" display="url" xr:uid="{8A9B7FA3-1928-41CA-87C6-541FA3F61702}"/>
-    <hyperlink ref="P31" r:id="rId27" display="url" xr:uid="{9D856677-C9BD-46E0-B856-5AE5200237C2}"/>
-    <hyperlink ref="P32" r:id="rId28" display="url" xr:uid="{0A3DB5F0-0282-4DB6-995C-109E7903A8F7}"/>
-    <hyperlink ref="P33" r:id="rId29" display="url" xr:uid="{4BD2E770-4F34-4266-B228-500F78BD7F04}"/>
-    <hyperlink ref="P34" r:id="rId30" display="url" xr:uid="{CBBD2ABE-8F9A-4DC9-B46F-C5010852EC83}"/>
-    <hyperlink ref="P35" r:id="rId31" display="url" xr:uid="{1C2CE604-88B0-4DFA-B6BF-D62A22203A96}"/>
-    <hyperlink ref="P36" r:id="rId32" display="url" xr:uid="{A60C9F95-C81B-4CBE-8D90-0A81A615F831}"/>
-    <hyperlink ref="P37" r:id="rId33" display="url" xr:uid="{915061B9-DC72-4F03-A1AE-E20FEA39C2C9}"/>
-    <hyperlink ref="P38" r:id="rId34" display="url" xr:uid="{496FD0BB-7104-4870-BDAC-C07F0F59B575}"/>
-    <hyperlink ref="P39" r:id="rId35" display="url" xr:uid="{12545ABE-5AA7-4C56-99BD-19E825C0BD91}"/>
-    <hyperlink ref="P40" r:id="rId36" display="url" xr:uid="{EDE87927-E26F-409D-AF6A-DDB9EF6349DA}"/>
-    <hyperlink ref="P41" r:id="rId37" display="url" xr:uid="{397ABB64-0DDB-4648-B72F-A91FDBE4A709}"/>
-    <hyperlink ref="P42" r:id="rId38" display="url" xr:uid="{DD03F2D1-9EFB-4142-A5B7-044C60B7C9BF}"/>
-    <hyperlink ref="P43" r:id="rId39" display="url" xr:uid="{EDE88620-BF02-48E6-9191-8C832B828CB2}"/>
-    <hyperlink ref="P44" r:id="rId40" display="url" xr:uid="{FE291AD4-F3C3-49E5-8076-78E5CB4B7FE0}"/>
-    <hyperlink ref="P45" r:id="rId41" display="url" xr:uid="{2215F9AD-C50B-46F2-952B-7B30EDB9A725}"/>
-    <hyperlink ref="P46" r:id="rId42" display="url" xr:uid="{839BB942-59B6-439E-8EA7-3AE905C8D838}"/>
-    <hyperlink ref="P47" r:id="rId43" display="url" xr:uid="{9895946F-43A6-40FF-8AF7-60815D71B767}"/>
-    <hyperlink ref="P49" r:id="rId44" display="url" xr:uid="{13E066E7-D6C7-4B0B-907A-CBA40F301990}"/>
+    <hyperlink ref="P29" r:id="rId24" display="url" xr:uid="{06A4437F-89A2-4876-AD94-331DFFE2053D}"/>
+    <hyperlink ref="P30" r:id="rId25" display="url" xr:uid="{8A9B7FA3-1928-41CA-87C6-541FA3F61702}"/>
+    <hyperlink ref="P31" r:id="rId26" display="url" xr:uid="{9D856677-C9BD-46E0-B856-5AE5200237C2}"/>
+    <hyperlink ref="P32" r:id="rId27" display="url" xr:uid="{0A3DB5F0-0282-4DB6-995C-109E7903A8F7}"/>
+    <hyperlink ref="P33" r:id="rId28" display="url" xr:uid="{4BD2E770-4F34-4266-B228-500F78BD7F04}"/>
+    <hyperlink ref="P34" r:id="rId29" display="url" xr:uid="{CBBD2ABE-8F9A-4DC9-B46F-C5010852EC83}"/>
+    <hyperlink ref="P35" r:id="rId30" display="url" xr:uid="{1C2CE604-88B0-4DFA-B6BF-D62A22203A96}"/>
+    <hyperlink ref="P36" r:id="rId31" display="url" xr:uid="{A60C9F95-C81B-4CBE-8D90-0A81A615F831}"/>
+    <hyperlink ref="P37" r:id="rId32" display="url" xr:uid="{915061B9-DC72-4F03-A1AE-E20FEA39C2C9}"/>
+    <hyperlink ref="P38" r:id="rId33" display="url" xr:uid="{496FD0BB-7104-4870-BDAC-C07F0F59B575}"/>
+    <hyperlink ref="P39" r:id="rId34" display="url" xr:uid="{12545ABE-5AA7-4C56-99BD-19E825C0BD91}"/>
+    <hyperlink ref="P40" r:id="rId35" display="url" xr:uid="{EDE87927-E26F-409D-AF6A-DDB9EF6349DA}"/>
+    <hyperlink ref="P41" r:id="rId36" display="url" xr:uid="{397ABB64-0DDB-4648-B72F-A91FDBE4A709}"/>
+    <hyperlink ref="P42" r:id="rId37" display="url" xr:uid="{DD03F2D1-9EFB-4142-A5B7-044C60B7C9BF}"/>
+    <hyperlink ref="P43" r:id="rId38" display="url" xr:uid="{EDE88620-BF02-48E6-9191-8C832B828CB2}"/>
+    <hyperlink ref="P44" r:id="rId39" display="url" xr:uid="{FE291AD4-F3C3-49E5-8076-78E5CB4B7FE0}"/>
+    <hyperlink ref="P45" r:id="rId40" display="url" xr:uid="{2215F9AD-C50B-46F2-952B-7B30EDB9A725}"/>
+    <hyperlink ref="P46" r:id="rId41" display="url" xr:uid="{839BB942-59B6-439E-8EA7-3AE905C8D838}"/>
+    <hyperlink ref="P47" r:id="rId42" display="url" xr:uid="{9895946F-43A6-40FF-8AF7-60815D71B767}"/>
+    <hyperlink ref="P49" r:id="rId43" display="url" xr:uid="{13E066E7-D6C7-4B0B-907A-CBA40F301990}"/>
+    <hyperlink ref="P28" r:id="rId44" xr:uid="{48BD8DD4-4E3B-486C-94DE-0EABB9874F27}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId45"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>